<commit_message>
Increased coverage to 410 projects
</commit_message>
<xml_diff>
--- a/testing/PIQUE_Projects/output/projects_auto.xlsx
+++ b/testing/PIQUE_Projects/output/projects_auto.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H351"/>
+  <dimension ref="A1:H411"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12384,6 +12384,2046 @@
         </is>
       </c>
     </row>
+    <row r="352">
+      <c r="A352" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/build-metrics-plugin</t>
+        </is>
+      </c>
+      <c r="B352" s="1" t="inlineStr">
+        <is>
+          <t>build-metrics-1.3</t>
+        </is>
+      </c>
+      <c r="C352" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D352" s="1" t="inlineStr">
+        <is>
+          <t>build-metrics-plugin-build-metrics-1.3</t>
+        </is>
+      </c>
+      <c r="E352" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F352" s="1" t="inlineStr"/>
+      <c r="G352" s="1" t="inlineStr"/>
+      <c r="H352" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/build-metrics-plugin/archive/refs/tags/build-metrics-1.3.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" s="1" t="inlineStr">
+        <is>
+          <t>spray/spray-json</t>
+        </is>
+      </c>
+      <c r="B353" s="1" t="inlineStr">
+        <is>
+          <t>v1.3.6</t>
+        </is>
+      </c>
+      <c r="C353" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D353" s="1" t="inlineStr">
+        <is>
+          <t>spray-json-1.3.6</t>
+        </is>
+      </c>
+      <c r="E353" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F353" s="1" t="inlineStr"/>
+      <c r="G353" s="1" t="inlineStr"/>
+      <c r="H353" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/spray/spray-json/archive/refs/tags/v1.3.6.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/stash-branch-parameters-plugin</t>
+        </is>
+      </c>
+      <c r="B354" s="1" t="inlineStr">
+        <is>
+          <t>StashBranchParameter-0.3.0</t>
+        </is>
+      </c>
+      <c r="C354" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D354" s="1" t="inlineStr">
+        <is>
+          <t>stash-branch-parameters-plugin-StashBranchParameter-0.3.0</t>
+        </is>
+      </c>
+      <c r="E354" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F354" s="1" t="inlineStr"/>
+      <c r="G354" s="1" t="inlineStr"/>
+      <c r="H354" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/stash-branch-parameters-plugin/archive/refs/tags/StashBranchParameter-0.3.0.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/threadfix-plugin</t>
+        </is>
+      </c>
+      <c r="B355" s="1" t="inlineStr">
+        <is>
+          <t>threadfix-1.5.4</t>
+        </is>
+      </c>
+      <c r="C355" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D355" s="1" t="inlineStr">
+        <is>
+          <t>threadfix-plugin-threadfix-1.5.4</t>
+        </is>
+      </c>
+      <c r="E355" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F355" s="1" t="inlineStr"/>
+      <c r="G355" s="1" t="inlineStr"/>
+      <c r="H355" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/threadfix-plugin/archive/refs/tags/threadfix-1.5.4.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/vmware-vrealize-orchestrator-plugin</t>
+        </is>
+      </c>
+      <c r="B356" s="2" t="inlineStr">
+        <is>
+          <t>vmware-vrealize-orchestrator-4.0.0</t>
+        </is>
+      </c>
+      <c r="C356" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D356" s="2" t="inlineStr">
+        <is>
+          <t>vmware-vrealize-orchestrator-plugin-vmware-vrealize-orchestrator-4.0.0</t>
+        </is>
+      </c>
+      <c r="E356" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F356" s="2" t="inlineStr"/>
+      <c r="G356" s="2" t="inlineStr"/>
+      <c r="H356" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/vmware-vrealize-orchestrator-plugin/archive/refs/tags/vmware-vrealize-orchestrator-4.0.0.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/squashtm-publisher-plugin</t>
+        </is>
+      </c>
+      <c r="B357" s="1" t="inlineStr">
+        <is>
+          <t>squashtm-publisher-1.0.0</t>
+        </is>
+      </c>
+      <c r="C357" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D357" s="1" t="inlineStr">
+        <is>
+          <t>squashtm-publisher-plugin-squashtm-publisher-1.0.0</t>
+        </is>
+      </c>
+      <c r="E357" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F357" s="1" t="inlineStr"/>
+      <c r="G357" s="1" t="inlineStr"/>
+      <c r="H357" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/squashtm-publisher-plugin/archive/refs/tags/squashtm-publisher-1.0.0.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/ontrack-plugin</t>
+        </is>
+      </c>
+      <c r="B358" s="2" t="inlineStr">
+        <is>
+          <t>ontrack-4.0.0</t>
+        </is>
+      </c>
+      <c r="C358" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D358" s="2" t="inlineStr">
+        <is>
+          <t>ontrack-plugin-ontrack-4.0.0</t>
+        </is>
+      </c>
+      <c r="E358" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F358" s="2" t="inlineStr"/>
+      <c r="G358" s="2" t="inlineStr"/>
+      <c r="H358" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/ontrack-plugin/archive/refs/tags/ontrack-4.0.0.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/agent-server-parameter-plugin</t>
+        </is>
+      </c>
+      <c r="B359" s="2" t="inlineStr">
+        <is>
+          <t>agent-server-parameter-1.1</t>
+        </is>
+      </c>
+      <c r="C359" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D359" s="2" t="inlineStr">
+        <is>
+          <t>agent-server-parameter-plugin-agent-server-parameter-1.1</t>
+        </is>
+      </c>
+      <c r="E359" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F359" s="2" t="inlineStr"/>
+      <c r="G359" s="2" t="inlineStr"/>
+      <c r="H359" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/agent-server-parameter-plugin/archive/refs/tags/agent-server-parameter-1.1.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/rest-list-parameter-plugin</t>
+        </is>
+      </c>
+      <c r="B360" s="2" t="inlineStr">
+        <is>
+          <t>344.v848a_89845169</t>
+        </is>
+      </c>
+      <c r="C360" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D360" s="2" t="inlineStr">
+        <is>
+          <t>rest-list-parameter-plugin-344.v848a_89845169</t>
+        </is>
+      </c>
+      <c r="E360" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F360" s="2" t="inlineStr"/>
+      <c r="G360" s="2" t="inlineStr"/>
+      <c r="H360" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/rest-list-parameter-plugin/archive/refs/tags/344.v848a_89845169.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/nested-view-plugin</t>
+        </is>
+      </c>
+      <c r="B361" s="2" t="inlineStr">
+        <is>
+          <t>nested-view-1.30</t>
+        </is>
+      </c>
+      <c r="C361" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D361" s="2" t="inlineStr">
+        <is>
+          <t>nested-view-plugin-nested-view-1.30</t>
+        </is>
+      </c>
+      <c r="E361" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F361" s="2" t="inlineStr"/>
+      <c r="G361" s="2" t="inlineStr"/>
+      <c r="H361" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/nested-view-plugin/archive/refs/tags/nested-view-1.30.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="1" t="inlineStr">
+        <is>
+          <t>alibaba/fastjson</t>
+        </is>
+      </c>
+      <c r="B362" s="1" t="inlineStr">
+        <is>
+          <t>1.2.83</t>
+        </is>
+      </c>
+      <c r="C362" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D362" s="1" t="inlineStr">
+        <is>
+          <t>fastjson-1.2.83</t>
+        </is>
+      </c>
+      <c r="E362" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F362" s="1" t="inlineStr"/>
+      <c r="G362" s="1" t="inlineStr"/>
+      <c r="H362" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/alibaba/fastjson/archive/refs/tags/1.2.83.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="2" t="inlineStr">
+        <is>
+          <t>erudika/para</t>
+        </is>
+      </c>
+      <c r="B363" s="2" t="inlineStr">
+        <is>
+          <t>v1.50.6</t>
+        </is>
+      </c>
+      <c r="C363" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D363" s="2" t="inlineStr">
+        <is>
+          <t>para-1.50.6</t>
+        </is>
+      </c>
+      <c r="E363" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F363" s="2" t="inlineStr"/>
+      <c r="G363" s="2" t="inlineStr"/>
+      <c r="H363" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/erudika/para/archive/refs/tags/v1.50.6.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="1" t="inlineStr">
+        <is>
+          <t>akka/akka-http</t>
+        </is>
+      </c>
+      <c r="B364" s="1" t="inlineStr">
+        <is>
+          <t>v10.7.1</t>
+        </is>
+      </c>
+      <c r="C364" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D364" s="1" t="inlineStr">
+        <is>
+          <t>akka-http-10.7.1</t>
+        </is>
+      </c>
+      <c r="E364" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F364" s="1" t="inlineStr"/>
+      <c r="G364" s="1" t="inlineStr"/>
+      <c r="H364" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/akka/akka-http/archive/refs/tags/v10.7.1.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/saml-plugin</t>
+        </is>
+      </c>
+      <c r="B365" s="2" t="inlineStr">
+        <is>
+          <t>4.525.v4f6a_7209447e</t>
+        </is>
+      </c>
+      <c r="C365" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D365" s="2" t="inlineStr">
+        <is>
+          <t>saml-plugin-4.525.v4f6a_7209447e</t>
+        </is>
+      </c>
+      <c r="E365" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F365" s="2" t="inlineStr"/>
+      <c r="G365" s="2" t="inlineStr"/>
+      <c r="H365" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/saml-plugin/archive/refs/tags/4.525.v4f6a_7209447e.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/nomad-plugin</t>
+        </is>
+      </c>
+      <c r="B366" s="2" t="inlineStr">
+        <is>
+          <t>v0.10.0</t>
+        </is>
+      </c>
+      <c r="C366" s="2" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="D366" s="2" t="inlineStr">
+        <is>
+          <t>nomad-plugin-0.10.0</t>
+        </is>
+      </c>
+      <c r="E366" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F366" s="2" t="inlineStr"/>
+      <c r="G366" s="2" t="inlineStr"/>
+      <c r="H366" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/nomad-plugin/archive/refs/tags/v0.10.0.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/urltrigger-plugin</t>
+        </is>
+      </c>
+      <c r="B367" s="1" t="inlineStr">
+        <is>
+          <t>urltrigger-0.47</t>
+        </is>
+      </c>
+      <c r="C367" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D367" s="1" t="inlineStr">
+        <is>
+          <t>urltrigger-plugin-urltrigger-0.47</t>
+        </is>
+      </c>
+      <c r="E367" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F367" s="1" t="inlineStr"/>
+      <c r="G367" s="1" t="inlineStr"/>
+      <c r="H367" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/urltrigger-plugin/archive/refs/tags/urltrigger-0.47.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/promoted-builds-plugin</t>
+        </is>
+      </c>
+      <c r="B368" s="2" t="inlineStr">
+        <is>
+          <t>992.va_00888f21b_74</t>
+        </is>
+      </c>
+      <c r="C368" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D368" s="2" t="inlineStr">
+        <is>
+          <t>promoted-builds-plugin-992.va_00888f21b_74</t>
+        </is>
+      </c>
+      <c r="E368" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F368" s="2" t="inlineStr"/>
+      <c r="G368" s="2" t="inlineStr"/>
+      <c r="H368" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/promoted-builds-plugin/archive/refs/tags/992.va_00888f21b_74.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/dependency-track-plugin</t>
+        </is>
+      </c>
+      <c r="B369" s="2" t="inlineStr">
+        <is>
+          <t>v6.0.1</t>
+        </is>
+      </c>
+      <c r="C369" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D369" s="2" t="inlineStr">
+        <is>
+          <t>dependency-track-plugin-6.0.1</t>
+        </is>
+      </c>
+      <c r="E369" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F369" s="2" t="inlineStr"/>
+      <c r="G369" s="2" t="inlineStr"/>
+      <c r="H369" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/dependency-track-plugin/archive/refs/tags/v6.0.1.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/build-with-parameters-plugin</t>
+        </is>
+      </c>
+      <c r="B370" s="2" t="inlineStr">
+        <is>
+          <t>76.v9382db_f78962</t>
+        </is>
+      </c>
+      <c r="C370" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D370" s="2" t="inlineStr">
+        <is>
+          <t>build-with-parameters-plugin-76.v9382db_f78962</t>
+        </is>
+      </c>
+      <c r="E370" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F370" s="2" t="inlineStr"/>
+      <c r="G370" s="2" t="inlineStr"/>
+      <c r="H370" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/build-with-parameters-plugin/archive/refs/tags/76.v9382db_f78962.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/extra-columns-plugin</t>
+        </is>
+      </c>
+      <c r="B371" s="2" t="inlineStr">
+        <is>
+          <t>extra-columns-1.27</t>
+        </is>
+      </c>
+      <c r="C371" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D371" s="2" t="inlineStr">
+        <is>
+          <t>extra-columns-plugin-extra-columns-1.27</t>
+        </is>
+      </c>
+      <c r="E371" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F371" s="2" t="inlineStr"/>
+      <c r="G371" s="2" t="inlineStr"/>
+      <c r="H371" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/extra-columns-plugin/archive/refs/tags/extra-columns-1.27.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/aws-credentials-plugin</t>
+        </is>
+      </c>
+      <c r="B372" s="2" t="inlineStr">
+        <is>
+          <t>245.v8a_1b_7c11a_94d</t>
+        </is>
+      </c>
+      <c r="C372" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D372" s="2" t="inlineStr">
+        <is>
+          <t>aws-credentials-plugin-245.v8a_1b_7c11a_94d</t>
+        </is>
+      </c>
+      <c r="E372" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F372" s="2" t="inlineStr"/>
+      <c r="G372" s="2" t="inlineStr"/>
+      <c r="H372" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/aws-credentials-plugin/archive/refs/tags/245.v8a_1b_7c11a_94d.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/matrix-auth-plugin</t>
+        </is>
+      </c>
+      <c r="B373" s="2" t="inlineStr">
+        <is>
+          <t>matrix-auth-3.2.6</t>
+        </is>
+      </c>
+      <c r="C373" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D373" s="2" t="inlineStr">
+        <is>
+          <t>matrix-auth-plugin-matrix-auth-3.2.6</t>
+        </is>
+      </c>
+      <c r="E373" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F373" s="2" t="inlineStr"/>
+      <c r="G373" s="2" t="inlineStr"/>
+      <c r="H373" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/matrix-auth-plugin/archive/refs/tags/matrix-auth-3.2.6.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/claim-plugin</t>
+        </is>
+      </c>
+      <c r="B374" s="2" t="inlineStr">
+        <is>
+          <t>599.v95c2f92e1c88</t>
+        </is>
+      </c>
+      <c r="C374" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D374" s="2" t="inlineStr">
+        <is>
+          <t>claim-plugin-599.v95c2f92e1c88</t>
+        </is>
+      </c>
+      <c r="E374" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F374" s="2" t="inlineStr"/>
+      <c r="G374" s="2" t="inlineStr"/>
+      <c r="H374" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/claim-plugin/archive/refs/tags/599.v95c2f92e1c88.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/chaos-monkey-plugin</t>
+        </is>
+      </c>
+      <c r="B375" s="1" t="inlineStr">
+        <is>
+          <t>chaos-monkey-0.3</t>
+        </is>
+      </c>
+      <c r="C375" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D375" s="1" t="inlineStr">
+        <is>
+          <t>chaos-monkey-plugin-chaos-monkey-0.3</t>
+        </is>
+      </c>
+      <c r="E375" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F375" s="1" t="inlineStr"/>
+      <c r="G375" s="1" t="inlineStr"/>
+      <c r="H375" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/chaos-monkey-plugin/archive/refs/tags/chaos-monkey-0.3.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/maven-release-cascade-plugin</t>
+        </is>
+      </c>
+      <c r="B376" s="1" t="inlineStr">
+        <is>
+          <t>maven-release-cascade-1.3.2</t>
+        </is>
+      </c>
+      <c r="C376" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D376" s="1" t="inlineStr">
+        <is>
+          <t>maven-release-cascade-plugin-maven-release-cascade-1.3.2</t>
+        </is>
+      </c>
+      <c r="E376" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F376" s="1" t="inlineStr"/>
+      <c r="G376" s="1" t="inlineStr"/>
+      <c r="H376" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/maven-release-cascade-plugin/archive/refs/tags/maven-release-cascade-1.3.2.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/lockable-resources-plugin</t>
+        </is>
+      </c>
+      <c r="B377" s="2" t="inlineStr">
+        <is>
+          <t>1349.v8b_ccb_c5487f7</t>
+        </is>
+      </c>
+      <c r="C377" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D377" s="2" t="inlineStr">
+        <is>
+          <t>lockable-resources-plugin-1349.v8b_ccb_c5487f7</t>
+        </is>
+      </c>
+      <c r="E377" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F377" s="2" t="inlineStr"/>
+      <c r="G377" s="2" t="inlineStr"/>
+      <c r="H377" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/lockable-resources-plugin/archive/refs/tags/1349.v8b_ccb_c5487f7.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/warnings-plugin</t>
+        </is>
+      </c>
+      <c r="B378" s="2" t="inlineStr">
+        <is>
+          <t>warnings-5.0.2</t>
+        </is>
+      </c>
+      <c r="C378" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D378" s="2" t="inlineStr">
+        <is>
+          <t>warnings-plugin-warnings-5.0.2</t>
+        </is>
+      </c>
+      <c r="E378" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F378" s="2" t="inlineStr"/>
+      <c r="G378" s="2" t="inlineStr"/>
+      <c r="H378" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/warnings-plugin/archive/refs/tags/warnings-5.0.2.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/selection-tasks-plugin</t>
+        </is>
+      </c>
+      <c r="B379" s="1" t="inlineStr">
+        <is>
+          <t>selection-tasks-plugin-1.0</t>
+        </is>
+      </c>
+      <c r="C379" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D379" s="1" t="inlineStr">
+        <is>
+          <t>selection-tasks-plugin-selection-tasks-plugin-1.0</t>
+        </is>
+      </c>
+      <c r="E379" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F379" s="1" t="inlineStr"/>
+      <c r="G379" s="1" t="inlineStr"/>
+      <c r="H379" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/selection-tasks-plugin/archive/refs/tags/selection-tasks-plugin-1.0.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/perfecto-plugin</t>
+        </is>
+      </c>
+      <c r="B380" s="2" t="inlineStr">
+        <is>
+          <t>perfecto-1.26</t>
+        </is>
+      </c>
+      <c r="C380" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D380" s="2" t="inlineStr">
+        <is>
+          <t>perfecto-plugin-perfecto-1.26</t>
+        </is>
+      </c>
+      <c r="E380" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F380" s="2" t="inlineStr"/>
+      <c r="G380" s="2" t="inlineStr"/>
+      <c r="H380" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/perfecto-plugin/archive/refs/tags/perfecto-1.26.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/mongodb-plugin</t>
+        </is>
+      </c>
+      <c r="B381" s="1" t="inlineStr">
+        <is>
+          <t>mongodb-1.3</t>
+        </is>
+      </c>
+      <c r="C381" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D381" s="1" t="inlineStr">
+        <is>
+          <t>mongodb-plugin-mongodb-1.3</t>
+        </is>
+      </c>
+      <c r="E381" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F381" s="1" t="inlineStr"/>
+      <c r="G381" s="1" t="inlineStr"/>
+      <c r="H381" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/mongodb-plugin/archive/refs/tags/mongodb-1.3.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/covcomplplot-plugin</t>
+        </is>
+      </c>
+      <c r="B382" s="1" t="inlineStr">
+        <is>
+          <t>covcomplplot-1.1.4</t>
+        </is>
+      </c>
+      <c r="C382" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D382" s="1" t="inlineStr">
+        <is>
+          <t>covcomplplot-plugin-covcomplplot-1.1.4</t>
+        </is>
+      </c>
+      <c r="E382" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F382" s="1" t="inlineStr"/>
+      <c r="G382" s="1" t="inlineStr"/>
+      <c r="H382" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/covcomplplot-plugin/archive/refs/tags/covcomplplot-1.1.4.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/soapui-pro-functional-testing-plugin</t>
+        </is>
+      </c>
+      <c r="B383" s="1" t="inlineStr">
+        <is>
+          <t>soapui-pro-functional-testing-1.11</t>
+        </is>
+      </c>
+      <c r="C383" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D383" s="1" t="inlineStr">
+        <is>
+          <t>soapui-pro-functional-testing-plugin-soapui-pro-functional-testing-1.11</t>
+        </is>
+      </c>
+      <c r="E383" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F383" s="1" t="inlineStr"/>
+      <c r="G383" s="1" t="inlineStr"/>
+      <c r="H383" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/soapui-pro-functional-testing-plugin/archive/refs/tags/soapui-pro-functional-testing-1.11.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/valgrind-plugin</t>
+        </is>
+      </c>
+      <c r="B384" s="1" t="inlineStr">
+        <is>
+          <t>valgrind-0.28</t>
+        </is>
+      </c>
+      <c r="C384" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D384" s="1" t="inlineStr">
+        <is>
+          <t>valgrind-plugin-valgrind-0.28</t>
+        </is>
+      </c>
+      <c r="E384" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F384" s="1" t="inlineStr"/>
+      <c r="G384" s="1" t="inlineStr"/>
+      <c r="H384" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/valgrind-plugin/archive/refs/tags/valgrind-0.28.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/flaky-test-handler-plugin</t>
+        </is>
+      </c>
+      <c r="B385" s="2" t="inlineStr">
+        <is>
+          <t>1.3.168.v9b_0b_fd020db_8</t>
+        </is>
+      </c>
+      <c r="C385" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D385" s="2" t="inlineStr">
+        <is>
+          <t>flaky-test-handler-plugin-1.3.168.v9b_0b_fd020db_8</t>
+        </is>
+      </c>
+      <c r="E385" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F385" s="2" t="inlineStr"/>
+      <c r="G385" s="2" t="inlineStr"/>
+      <c r="H385" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/flaky-test-handler-plugin/archive/refs/tags/1.3.168.v9b_0b_fd020db_8.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/vncrecorder-plugin</t>
+        </is>
+      </c>
+      <c r="B386" s="1" t="inlineStr">
+        <is>
+          <t>vncrecorder-1.26</t>
+        </is>
+      </c>
+      <c r="C386" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D386" s="1" t="inlineStr">
+        <is>
+          <t>vncrecorder-plugin-vncrecorder-1.26</t>
+        </is>
+      </c>
+      <c r="E386" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F386" s="1" t="inlineStr"/>
+      <c r="G386" s="1" t="inlineStr"/>
+      <c r="H386" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/vncrecorder-plugin/archive/refs/tags/vncrecorder-1.26.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/swarm-plugin</t>
+        </is>
+      </c>
+      <c r="B387" s="2" t="inlineStr">
+        <is>
+          <t>swarm-plugin-3.49</t>
+        </is>
+      </c>
+      <c r="C387" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D387" s="2" t="inlineStr">
+        <is>
+          <t>swarm-plugin-swarm-plugin-3.49</t>
+        </is>
+      </c>
+      <c r="E387" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F387" s="2" t="inlineStr"/>
+      <c r="G387" s="2" t="inlineStr"/>
+      <c r="H387" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/swarm-plugin/archive/refs/tags/swarm-plugin-3.49.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/echarts-api-plugin</t>
+        </is>
+      </c>
+      <c r="B388" s="2" t="inlineStr">
+        <is>
+          <t>v5.6.0-4</t>
+        </is>
+      </c>
+      <c r="C388" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D388" s="2" t="inlineStr">
+        <is>
+          <t>echarts-api-plugin-5.6.0-4</t>
+        </is>
+      </c>
+      <c r="E388" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F388" s="2" t="inlineStr"/>
+      <c r="G388" s="2" t="inlineStr"/>
+      <c r="H388" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/echarts-api-plugin/archive/refs/tags/v5.6.0-4.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/fitnesse-plugin</t>
+        </is>
+      </c>
+      <c r="B389" s="2" t="inlineStr">
+        <is>
+          <t>fitnesse-1.36</t>
+        </is>
+      </c>
+      <c r="C389" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D389" s="2" t="inlineStr">
+        <is>
+          <t>fitnesse-plugin-fitnesse-1.36</t>
+        </is>
+      </c>
+      <c r="E389" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F389" s="2" t="inlineStr"/>
+      <c r="G389" s="2" t="inlineStr"/>
+      <c r="H389" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/fitnesse-plugin/archive/refs/tags/fitnesse-1.36.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/rapiddeploy-plugin</t>
+        </is>
+      </c>
+      <c r="B390" s="2" t="inlineStr">
+        <is>
+          <t>rapiddeploy-jenkins-4.9</t>
+        </is>
+      </c>
+      <c r="C390" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D390" s="2" t="inlineStr">
+        <is>
+          <t>rapiddeploy-plugin-rapiddeploy-jenkins-4.9</t>
+        </is>
+      </c>
+      <c r="E390" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F390" s="2" t="inlineStr"/>
+      <c r="G390" s="2" t="inlineStr"/>
+      <c r="H390" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/rapiddeploy-plugin/archive/refs/tags/rapiddeploy-jenkins-4.9.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/skytap-cloud-plugin</t>
+        </is>
+      </c>
+      <c r="B391" s="1" t="inlineStr">
+        <is>
+          <t>skytap-2.07</t>
+        </is>
+      </c>
+      <c r="C391" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D391" s="1" t="inlineStr">
+        <is>
+          <t>skytap-cloud-plugin-skytap-2.07</t>
+        </is>
+      </c>
+      <c r="E391" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F391" s="1" t="inlineStr"/>
+      <c r="G391" s="1" t="inlineStr"/>
+      <c r="H391" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/skytap-cloud-plugin/archive/refs/tags/skytap-2.07.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/deployhub-plugin</t>
+        </is>
+      </c>
+      <c r="B392" s="2" t="inlineStr">
+        <is>
+          <t>deployhub-8.0.14</t>
+        </is>
+      </c>
+      <c r="C392" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D392" s="2" t="inlineStr">
+        <is>
+          <t>deployhub-plugin-deployhub-8.0.14</t>
+        </is>
+      </c>
+      <c r="E392" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F392" s="2" t="inlineStr"/>
+      <c r="G392" s="2" t="inlineStr"/>
+      <c r="H392" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/deployhub-plugin/archive/refs/tags/deployhub-8.0.14.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/cobertura-plugin</t>
+        </is>
+      </c>
+      <c r="B393" s="2" t="inlineStr">
+        <is>
+          <t>cobertura-1.17</t>
+        </is>
+      </c>
+      <c r="C393" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D393" s="2" t="inlineStr">
+        <is>
+          <t>cobertura-plugin-cobertura-1.17</t>
+        </is>
+      </c>
+      <c r="E393" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F393" s="2" t="inlineStr"/>
+      <c r="G393" s="2" t="inlineStr"/>
+      <c r="H393" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/cobertura-plugin/archive/refs/tags/cobertura-1.17.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/harvest-plugin</t>
+        </is>
+      </c>
+      <c r="B394" s="1" t="inlineStr">
+        <is>
+          <t>harvest-0.5.1</t>
+        </is>
+      </c>
+      <c r="C394" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D394" s="1" t="inlineStr">
+        <is>
+          <t>harvest-plugin-harvest-0.5.1</t>
+        </is>
+      </c>
+      <c r="E394" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F394" s="1" t="inlineStr"/>
+      <c r="G394" s="1" t="inlineStr"/>
+      <c r="H394" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/harvest-plugin/archive/refs/tags/harvest-0.5.1.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/debian-package-builder-plugin</t>
+        </is>
+      </c>
+      <c r="B395" s="1" t="inlineStr">
+        <is>
+          <t>debian-package-builder-1.6.17</t>
+        </is>
+      </c>
+      <c r="C395" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D395" s="1" t="inlineStr">
+        <is>
+          <t>debian-package-builder-plugin-debian-package-builder-1.6.17</t>
+        </is>
+      </c>
+      <c r="E395" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F395" s="1" t="inlineStr"/>
+      <c r="G395" s="1" t="inlineStr"/>
+      <c r="H395" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/debian-package-builder-plugin/archive/refs/tags/debian-package-builder-1.6.17.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/google-kubernetes-engine-plugin</t>
+        </is>
+      </c>
+      <c r="B396" s="2" t="inlineStr">
+        <is>
+          <t>0.436.v0064b_4a_da_a_7a_</t>
+        </is>
+      </c>
+      <c r="C396" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D396" s="2" t="inlineStr">
+        <is>
+          <t>google-kubernetes-engine-plugin-0.436.v0064b_4a_da_a_7a_</t>
+        </is>
+      </c>
+      <c r="E396" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F396" s="2" t="inlineStr"/>
+      <c r="G396" s="2" t="inlineStr"/>
+      <c r="H396" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/google-kubernetes-engine-plugin/archive/refs/tags/0.436.v0064b_4a_da_a_7a_.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/sounds-plugin</t>
+        </is>
+      </c>
+      <c r="B397" s="1" t="inlineStr">
+        <is>
+          <t>sounds-0.7</t>
+        </is>
+      </c>
+      <c r="C397" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D397" s="1" t="inlineStr">
+        <is>
+          <t>sounds-plugin-sounds-0.7</t>
+        </is>
+      </c>
+      <c r="E397" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F397" s="1" t="inlineStr"/>
+      <c r="G397" s="1" t="inlineStr"/>
+      <c r="H397" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/sounds-plugin/archive/refs/tags/sounds-0.7.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/redgate-sql-ci-plugin</t>
+        </is>
+      </c>
+      <c r="B398" s="2" t="inlineStr">
+        <is>
+          <t>redgate-sql-ci-2.0.8</t>
+        </is>
+      </c>
+      <c r="C398" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D398" s="2" t="inlineStr">
+        <is>
+          <t>redgate-sql-ci-plugin-redgate-sql-ci-2.0.8</t>
+        </is>
+      </c>
+      <c r="E398" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F398" s="2" t="inlineStr"/>
+      <c r="G398" s="2" t="inlineStr"/>
+      <c r="H398" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/redgate-sql-ci-plugin/archive/refs/tags/redgate-sql-ci-2.0.8.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/google-compute-engine-plugin</t>
+        </is>
+      </c>
+      <c r="B399" s="2" t="inlineStr">
+        <is>
+          <t>4.683.v0ce26579a_ee7</t>
+        </is>
+      </c>
+      <c r="C399" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D399" s="2" t="inlineStr">
+        <is>
+          <t>google-compute-engine-plugin-4.683.v0ce26579a_ee7</t>
+        </is>
+      </c>
+      <c r="E399" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F399" s="2" t="inlineStr"/>
+      <c r="G399" s="2" t="inlineStr"/>
+      <c r="H399" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/google-compute-engine-plugin/archive/refs/tags/4.683.v0ce26579a_ee7.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" s="1" t="inlineStr">
+        <is>
+          <t>mulesoft/mule</t>
+        </is>
+      </c>
+      <c r="B400" s="1" t="inlineStr">
+        <is>
+          <t>mule-4.3.0-rc1</t>
+        </is>
+      </c>
+      <c r="C400" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D400" s="1" t="inlineStr">
+        <is>
+          <t>mule-mule-4.3.0-rc1</t>
+        </is>
+      </c>
+      <c r="E400" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F400" s="1" t="inlineStr"/>
+      <c r="G400" s="1" t="inlineStr"/>
+      <c r="H400" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/mulesoft/mule/archive/refs/tags/mule-4.3.0-rc1.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" s="1" t="inlineStr">
+        <is>
+          <t>koral--/android-gif-drawable</t>
+        </is>
+      </c>
+      <c r="B401" s="1" t="inlineStr">
+        <is>
+          <t>v1.2.29</t>
+        </is>
+      </c>
+      <c r="C401" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D401" s="1" t="inlineStr">
+        <is>
+          <t>android-gif-drawable-1.2.29</t>
+        </is>
+      </c>
+      <c r="E401" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F401" s="1" t="inlineStr"/>
+      <c r="G401" s="1" t="inlineStr"/>
+      <c r="H401" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/koral--/android-gif-drawable/archive/refs/tags/v1.2.29.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" s="1" t="inlineStr">
+        <is>
+          <t>jenkinsci/violation-comments-to-gitlab-plugin</t>
+        </is>
+      </c>
+      <c r="B402" s="1" t="inlineStr">
+        <is>
+          <t>violation-comments-to-gitlab-1.1</t>
+        </is>
+      </c>
+      <c r="C402" s="1" t="inlineStr">
+        <is>
+          <t>DNB</t>
+        </is>
+      </c>
+      <c r="D402" s="1" t="inlineStr">
+        <is>
+          <t>violation-comments-to-gitlab-plugin-violation-comments-to-gitlab-1.1</t>
+        </is>
+      </c>
+      <c r="E402" s="1" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="F402" s="1" t="inlineStr"/>
+      <c r="G402" s="1" t="inlineStr"/>
+      <c r="H402" s="1" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/violation-comments-to-gitlab-plugin/archive/refs/tags/violation-comments-to-gitlab-1.1.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" s="2" t="inlineStr">
+        <is>
+          <t>gradle/gradle</t>
+        </is>
+      </c>
+      <c r="B403" s="2" t="inlineStr">
+        <is>
+          <t>v8.14.0</t>
+        </is>
+      </c>
+      <c r="C403" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D403" s="2" t="inlineStr">
+        <is>
+          <t>gradle-8.14.0</t>
+        </is>
+      </c>
+      <c r="E403" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F403" s="2" t="inlineStr"/>
+      <c r="G403" s="2" t="inlineStr"/>
+      <c r="H403" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/gradle/gradle/archive/refs/tags/v8.14.0.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/mask-passwords-plugin</t>
+        </is>
+      </c>
+      <c r="B404" s="2" t="inlineStr">
+        <is>
+          <t>188.v66e477dcb_24a_</t>
+        </is>
+      </c>
+      <c r="C404" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D404" s="2" t="inlineStr">
+        <is>
+          <t>mask-passwords-plugin-188.v66e477dcb_24a_</t>
+        </is>
+      </c>
+      <c r="E404" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F404" s="2" t="inlineStr"/>
+      <c r="G404" s="2" t="inlineStr"/>
+      <c r="H404" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/mask-passwords-plugin/archive/refs/tags/188.v66e477dcb_24a_.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/docker-plugin</t>
+        </is>
+      </c>
+      <c r="B405" s="2" t="inlineStr">
+        <is>
+          <t>1274.vc0203fdf2e74</t>
+        </is>
+      </c>
+      <c r="C405" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D405" s="2" t="inlineStr">
+        <is>
+          <t>docker-plugin-1274.vc0203fdf2e74</t>
+        </is>
+      </c>
+      <c r="E405" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F405" s="2" t="inlineStr"/>
+      <c r="G405" s="2" t="inlineStr"/>
+      <c r="H405" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/docker-plugin/archive/refs/tags/1274.vc0203fdf2e74.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/token-macro-plugin</t>
+        </is>
+      </c>
+      <c r="B406" s="2" t="inlineStr">
+        <is>
+          <t>444.v52de7e9c573d</t>
+        </is>
+      </c>
+      <c r="C406" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D406" s="2" t="inlineStr">
+        <is>
+          <t>token-macro-plugin-444.v52de7e9c573d</t>
+        </is>
+      </c>
+      <c r="E406" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F406" s="2" t="inlineStr"/>
+      <c r="G406" s="2" t="inlineStr"/>
+      <c r="H406" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/token-macro-plugin/archive/refs/tags/444.v52de7e9c573d.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/credentials-plugin</t>
+        </is>
+      </c>
+      <c r="B407" s="2" t="inlineStr">
+        <is>
+          <t>1415.v831096eb_5534</t>
+        </is>
+      </c>
+      <c r="C407" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D407" s="2" t="inlineStr">
+        <is>
+          <t>credentials-plugin-1415.v831096eb_5534</t>
+        </is>
+      </c>
+      <c r="E407" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F407" s="2" t="inlineStr"/>
+      <c r="G407" s="2" t="inlineStr"/>
+      <c r="H407" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/credentials-plugin/archive/refs/tags/1415.v831096eb_5534.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" s="2" t="inlineStr">
+        <is>
+          <t>jenkinsci/windows-slaves-plugin</t>
+        </is>
+      </c>
+      <c r="B408" s="2" t="inlineStr">
+        <is>
+          <t>windows-slaves-1.8</t>
+        </is>
+      </c>
+      <c r="C408" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D408" s="2" t="inlineStr">
+        <is>
+          <t>windows-slaves-plugin-windows-slaves-1.8</t>
+        </is>
+      </c>
+      <c r="E408" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F408" s="2" t="inlineStr"/>
+      <c r="G408" s="2" t="inlineStr"/>
+      <c r="H408" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/jenkinsci/windows-slaves-plugin/archive/refs/tags/windows-slaves-1.8.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" s="2" t="inlineStr">
+        <is>
+          <t>apache/sling-org-apache-sling-auth-core</t>
+        </is>
+      </c>
+      <c r="B409" s="2" t="inlineStr">
+        <is>
+          <t>org.apache.sling.auth.core-1.7.0</t>
+        </is>
+      </c>
+      <c r="C409" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D409" s="2" t="inlineStr">
+        <is>
+          <t>sling-org-apache-sling-auth-core-org.apache.sling.auth.core-1.7.0</t>
+        </is>
+      </c>
+      <c r="E409" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F409" s="2" t="inlineStr"/>
+      <c r="G409" s="2" t="inlineStr"/>
+      <c r="H409" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/apache/sling-org-apache-sling-auth-core/archive/refs/tags/org.apache.sling.auth.core-1.7.0.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" s="2" t="inlineStr">
+        <is>
+          <t>opendaylight/openflowplugin</t>
+        </is>
+      </c>
+      <c r="B410" s="2" t="inlineStr">
+        <is>
+          <t>release/scandium-sr2</t>
+        </is>
+      </c>
+      <c r="C410" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D410" s="2" t="inlineStr">
+        <is>
+          <t>openflowplugin-release-scandium-sr2</t>
+        </is>
+      </c>
+      <c r="E410" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F410" s="2" t="inlineStr"/>
+      <c r="G410" s="2" t="inlineStr"/>
+      <c r="H410" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/opendaylight/openflowplugin/archive/refs/tags/release/scandium-sr2.zip</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" s="2" t="inlineStr">
+        <is>
+          <t>apache/sling-org-apache-sling-xss</t>
+        </is>
+      </c>
+      <c r="B411" s="2" t="inlineStr">
+        <is>
+          <t>org.apache.sling.xss-2.4.6</t>
+        </is>
+      </c>
+      <c r="C411" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D411" s="2" t="inlineStr">
+        <is>
+          <t>sling-org-apache-sling-xss-org.apache.sling.xss-2.4.6</t>
+        </is>
+      </c>
+      <c r="E411" s="2" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="F411" s="2" t="inlineStr"/>
+      <c r="G411" s="2" t="inlineStr"/>
+      <c r="H411" s="2" t="inlineStr">
+        <is>
+          <t>https://github.com/apache/sling-org-apache-sling-xss/archive/refs/tags/org.apache.sling.xss-2.4.6.zip</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>